<commit_message>
data updated at 12 Dec 11AM
</commit_message>
<xml_diff>
--- a/Retailers Ledger/AGNOOR.xlsx
+++ b/Retailers Ledger/AGNOOR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830" firstSheet="3" activeTab="5"/>
+    <workbookView windowWidth="20490" windowHeight="7830" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pawan &amp; Ravi - (660604868)" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="20">
   <si>
     <t>pawan and ravi telicom-(660604868)</t>
   </si>
@@ -89,10 +89,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -109,6 +109,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -116,11 +132,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -132,17 +148,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,23 +201,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,9 +224,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,50 +246,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -280,13 +280,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,37 +322,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,127 +454,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,6 +483,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -498,26 +507,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -555,19 +551,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -576,15 +576,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -594,134 +594,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -759,9 +759,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1086,7 +1083,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1101,11 +1098,12 @@
     <col min="16383" max="16384" width="9.14285714285714" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:6">
       <c r="A2" s="5" t="s">
@@ -1327,26 +1325,26 @@
     <row r="24" s="1" customFormat="1"/>
     <row r="25" s="1" customFormat="1"/>
     <row r="26" s="1" customFormat="1"/>
-    <row r="27" s="13" customFormat="1"/>
-    <row r="28" s="13" customFormat="1"/>
-    <row r="29" s="13" customFormat="1"/>
-    <row r="30" s="13" customFormat="1"/>
-    <row r="31" s="13" customFormat="1"/>
-    <row r="32" s="13" customFormat="1"/>
-    <row r="33" s="13" customFormat="1"/>
-    <row r="34" s="13" customFormat="1"/>
-    <row r="35" s="13" customFormat="1"/>
-    <row r="36" s="13" customFormat="1"/>
-    <row r="37" s="13" customFormat="1"/>
-    <row r="38" s="13" customFormat="1"/>
+    <row r="27" s="3" customFormat="1"/>
+    <row r="28" s="3" customFormat="1"/>
+    <row r="29" s="3" customFormat="1"/>
+    <row r="30" s="3" customFormat="1"/>
+    <row r="31" s="3" customFormat="1"/>
+    <row r="32" s="3" customFormat="1"/>
+    <row r="33" s="3" customFormat="1"/>
+    <row r="34" s="3" customFormat="1"/>
+    <row r="35" s="3" customFormat="1"/>
+    <row r="36" s="3" customFormat="1"/>
+    <row r="37" s="3" customFormat="1"/>
+    <row r="38" s="3" customFormat="1"/>
     <row r="39" s="1" customFormat="1"/>
     <row r="40" s="1" customFormat="1"/>
     <row r="41" s="1" customFormat="1"/>
-    <row r="42" s="13" customFormat="1"/>
-    <row r="43" s="13" customFormat="1"/>
-    <row r="44" s="13" customFormat="1"/>
-    <row r="45" s="13" customFormat="1"/>
-    <row r="46" s="13" customFormat="1"/>
+    <row r="42" s="3" customFormat="1"/>
+    <row r="43" s="3" customFormat="1"/>
+    <row r="44" s="3" customFormat="1"/>
+    <row r="45" s="3" customFormat="1"/>
+    <row r="46" s="3" customFormat="1"/>
     <row r="47" s="1" customFormat="1" spans="1:1">
       <c r="A47" s="6"/>
     </row>
@@ -1354,18 +1352,18 @@
       <c r="A48" s="6"/>
     </row>
     <row r="49" s="1" customFormat="1"/>
-    <row r="50" s="13" customFormat="1"/>
-    <row r="51" s="13" customFormat="1"/>
-    <row r="52" s="13" customFormat="1"/>
-    <row r="53" s="13" customFormat="1"/>
+    <row r="50" s="3" customFormat="1"/>
+    <row r="51" s="3" customFormat="1"/>
+    <row r="52" s="3" customFormat="1"/>
+    <row r="53" s="3" customFormat="1"/>
     <row r="54" s="1" customFormat="1" spans="1:1">
       <c r="A54" s="6"/>
     </row>
     <row r="55" s="1" customFormat="1"/>
     <row r="56" s="1" customFormat="1"/>
-    <row r="57" s="13" customFormat="1"/>
-    <row r="58" s="13" customFormat="1"/>
-    <row r="59" s="13" customFormat="1"/>
+    <row r="57" s="3" customFormat="1"/>
+    <row r="58" s="3" customFormat="1"/>
+    <row r="59" s="3" customFormat="1"/>
     <row r="60" s="1" customFormat="1" spans="1:1">
       <c r="A60" s="6"/>
     </row>
@@ -1375,7 +1373,8 @@
       <c r="A63" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="A3:C3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1389,7 +1388,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1825,10 +1824,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="$A14:$XFD14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -2028,6 +2027,20 @@
       </c>
       <c r="E14" s="3">
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="7">
+        <v>44176</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5200</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
@@ -2154,7 +2167,6 @@
       <c r="A8" s="7">
         <v>44175</v>
       </c>
-      <c r="B8" s="3"/>
       <c r="C8" s="3">
         <v>1000</v>
       </c>
@@ -2180,7 +2192,7 @@
   <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>